<commit_message>
all files checked in
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D0B1FF-9A94-44A3-998B-ED457A10DE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A31510-67A6-4C1E-8E66-8329BF4ABDAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIDBusiness" sheetId="1" r:id="rId1"/>
     <sheet name="CIDCompany" sheetId="3" r:id="rId2"/>
     <sheet name="CIDWatchlist" sheetId="4" r:id="rId3"/>
     <sheet name="LawlinkCompany" sheetId="5" r:id="rId4"/>
-    <sheet name="LawlinkDirector" sheetId="2" r:id="rId5"/>
+    <sheet name="LawlinkCIDDirector" sheetId="2" r:id="rId5"/>
     <sheet name="LawlinkWatchlist" sheetId="6" r:id="rId6"/>
     <sheet name="CIDLinksCheck" sheetId="7" r:id="rId7"/>
     <sheet name="LawlinkLinksCheck" sheetId="8" r:id="rId8"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="51">
   <si>
     <t>SKY AIRCRAFT B62694 LIMITED</t>
   </si>
@@ -173,13 +173,25 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>sanuat9</t>
+  </si>
+  <si>
+    <t>testref1</t>
+  </si>
+  <si>
+    <t>testref3</t>
+  </si>
+  <si>
+    <t>myreff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +203,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -822,6 +840,113 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1918994</v>
+      </c>
+      <c r="E1">
+        <v>11702552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2006686</v>
+      </c>
+      <c r="E2">
+        <v>16577161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2514484</v>
+      </c>
+      <c r="E3">
+        <v>438966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2514484</v>
+      </c>
+      <c r="E4">
+        <v>12463394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2514487</v>
+      </c>
+      <c r="E5">
+        <v>13898333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40037B92-8231-4568-A2BB-D8ACA631EA53}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
@@ -835,185 +960,78 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1">
-        <v>1918994</v>
-      </c>
-      <c r="E1">
-        <v>11702552</v>
+        <v>123108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2006686</v>
-      </c>
-      <c r="E2">
-        <v>16577161</v>
+        <v>192234</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2514484</v>
-      </c>
-      <c r="E3">
-        <v>438966</v>
+        <v>473446</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>2514484</v>
-      </c>
-      <c r="E4">
-        <v>12463394</v>
+        <v>685971</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2514487</v>
-      </c>
-      <c r="E5">
-        <v>13898333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40037B92-8231-4568-A2BB-D8ACA631EA53}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>123108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>192234</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>473446</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>685971</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1143,7 +1161,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,10 +1174,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1173,10 +1191,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1190,10 +1208,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1207,10 +1225,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1224,10 +1242,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1247,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2B0E35-2010-4DD0-A2D9-77380A65080C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1278,7 @@
     <col min="3" max="3" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1270,8 +1288,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1281,8 +1302,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1292,8 +1316,12 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>